<commit_message>
pvrp -> tr support
didn't really get anywhere from last time around
</commit_message>
<xml_diff>
--- a/data/PVRP/results/All_Short_Solutions.xlsx
+++ b/data/PVRP/results/All_Short_Solutions.xlsx
@@ -9,12 +9,13 @@
     <sheet name="pr4.xlsx" r:id="rId3" sheetId="1"/>
     <sheet name="pr6.xlsx" r:id="rId4" sheetId="2"/>
     <sheet name="p14.xlsx" r:id="rId5" sheetId="3"/>
+    <sheet name="p1.xlsx" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
   <si>
     <t>Filename</t>
   </si>
@@ -53,6 +54,12 @@
   </si>
   <si>
     <t>p14.xlsx</t>
+  </si>
+  <si>
+    <t>SmallestPolarAngleShortestDistToDepot</t>
+  </si>
+  <si>
+    <t>p1.xlsx</t>
   </si>
 </sst>
 </file>
@@ -4942,7 +4949,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
@@ -4989,16 +4996,16 @@
         <v>0.0</v>
       </c>
       <c r="F7" t="n">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
       <c r="G7" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="H7" t="n">
-        <v>7.0</v>
+        <v>19.0</v>
       </c>
       <c r="I7" t="n">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="J7" t="n">
         <v>1.0</v>
@@ -5018,27 +5025,369 @@
         <v>1.0</v>
       </c>
       <c r="D8" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D9" t="n">
         <v>15.0</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E8" t="n">
         <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G8" t="n">
-        <v>9.0</v>
+        <v>35.0</v>
       </c>
       <c r="H8" t="n">
         <v>3.0</v>
       </c>
       <c r="I8" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="M8" t="n">
         <v>13.0</v>
       </c>
-      <c r="J8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="N8" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="Q8" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -5047,13 +5396,13 @@
         <v>0.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" t="n">
         <v>2.0</v>
       </c>
       <c r="D9" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="E9" t="n">
         <v>0.0</v>
@@ -5062,18 +5411,30 @@
         <v>7.0</v>
       </c>
       <c r="G9" t="n">
-        <v>11.0</v>
+        <v>48.0</v>
       </c>
       <c r="H9" t="n">
-        <v>18.0</v>
+        <v>16.0</v>
       </c>
       <c r="I9" t="n">
-        <v>3.0</v>
+        <v>34.0</v>
       </c>
       <c r="J9" t="n">
-        <v>1.0</v>
+        <v>49.0</v>
       </c>
       <c r="K9" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="O9" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -5082,33 +5443,39 @@
         <v>0.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C10" t="n">
         <v>3.0</v>
       </c>
       <c r="D10" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" t="n">
         <v>0.0</v>
       </c>
       <c r="F10" t="n">
-        <v>14.0</v>
+        <v>25.0</v>
       </c>
       <c r="G10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="J10" t="n">
         <v>9.0</v>
       </c>
-      <c r="H10" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>1.0</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="M10" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -5117,33 +5484,51 @@
         <v>0.0</v>
       </c>
       <c r="B11" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C11" t="n">
         <v>4.0</v>
       </c>
       <c r="D11" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="E11" t="n">
         <v>0.0</v>
       </c>
       <c r="F11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="M11" t="n">
         <v>20.0</v>
       </c>
-      <c r="G11" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="H11" t="n">
+      <c r="N11" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="O11" t="n">
         <v>8.0</v>
       </c>
-      <c r="I11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="K11" t="n">
+      <c r="P11" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="Q11" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -5152,103 +5537,54 @@
         <v>0.0</v>
       </c>
       <c r="B12" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C12" t="n">
         <v>5.0</v>
       </c>
       <c r="D12" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="E12" t="n">
         <v>0.0</v>
       </c>
       <c r="F12" t="n">
-        <v>6.0</v>
+        <v>43.0</v>
       </c>
       <c r="G12" t="n">
-        <v>10.0</v>
+        <v>22.0</v>
       </c>
       <c r="H12" t="n">
-        <v>4.0</v>
+        <v>28.0</v>
       </c>
       <c r="I12" t="n">
-        <v>16.0</v>
+        <v>36.0</v>
       </c>
       <c r="J12" t="n">
         <v>2.0</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B13" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="G13" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="Q12" t="n">
         <v>12.0</v>
       </c>
-      <c r="H13" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B14" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="K14" t="n">
+      <c r="R12" t="n">
         <v>-1.0</v>
       </c>
     </row>

</xml_diff>